<commit_message>
[add] added analyze and k-means file
</commit_message>
<xml_diff>
--- a/Answer-Data.xlsx
+++ b/Answer-Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pan/Documents/01_University/02_Research/Working-Directory/eye-tracking-software/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC_User\iCloudDrive\Documents\01_University\02_Research\Working-Directory\eye-tracking-software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BFD6464-F722-184A-B745-CB59E74CD3C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D201D5D8-219D-4C77-84C5-7AFDCBA3E483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="660" windowWidth="38080" windowHeight="19560" xr2:uid="{65F65776-174E-4145-8CCF-AA6B8A50F68A}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{65F65776-174E-4145-8CCF-AA6B8A50F68A}"/>
   </bookViews>
   <sheets>
     <sheet name="1st" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="23">
   <si>
     <t>English</t>
   </si>
@@ -117,16 +117,44 @@
     </rPh>
     <phoneticPr fontId="2"/>
   </si>
+  <si>
+    <t>J1</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>elbow</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>BIC</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>Silhouette</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>J2</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>J3</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="2"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -138,7 +166,7 @@
     </font>
     <font>
       <sz val="6"/>
-      <name val="Aptos Narrow"/>
+      <name val="游ゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -253,7 +281,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -269,7 +297,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -585,26 +613,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60C853D4-11AD-448C-900A-323815755F36}">
-  <dimension ref="A1:AM37"/>
+  <dimension ref="A1:AP37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AB15" sqref="AB15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="10" style="3" customWidth="1"/>
-    <col min="2" max="3" width="4.1640625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="6.1640625" style="14" customWidth="1"/>
-    <col min="5" max="24" width="4.33203125" style="2" customWidth="1"/>
-    <col min="25" max="25" width="4.1640625" style="3" customWidth="1"/>
-    <col min="26" max="26" width="10" style="3" customWidth="1"/>
-    <col min="27" max="28" width="4.1640625" style="3" customWidth="1"/>
-    <col min="29" max="29" width="6.1640625" style="3" customWidth="1"/>
-    <col min="30" max="39" width="4.33203125" style="4" customWidth="1"/>
+    <col min="2" max="3" width="4.125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="6.125" style="14" customWidth="1"/>
+    <col min="5" max="24" width="4.375" style="2" customWidth="1"/>
+    <col min="25" max="25" width="4.125" style="3" customWidth="1"/>
+    <col min="26" max="29" width="10" style="3" customWidth="1"/>
+    <col min="30" max="31" width="4.125" style="3" customWidth="1"/>
+    <col min="32" max="32" width="6.125" style="3" customWidth="1"/>
+    <col min="33" max="42" width="4.375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" s="8" customFormat="1" ht="19.5" customHeight="1">
+    <row r="1" spans="1:42" s="8" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
@@ -640,32 +668,35 @@
       <c r="W1" s="17"/>
       <c r="X1" s="17"/>
       <c r="Y1" s="5"/>
-      <c r="Z1" s="5" t="s">
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5"/>
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="AA1" s="5" t="s">
+      <c r="AD1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="AB1" s="5" t="s">
+      <c r="AE1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="AC1" s="15" t="s">
+      <c r="AF1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="AD1" s="18" t="s">
+      <c r="AG1" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="AE1" s="18"/>
-      <c r="AF1" s="18"/>
-      <c r="AG1" s="18"/>
       <c r="AH1" s="18"/>
       <c r="AI1" s="18"/>
       <c r="AJ1" s="18"/>
       <c r="AK1" s="18"/>
       <c r="AL1" s="18"/>
       <c r="AM1" s="18"/>
+      <c r="AN1" s="18"/>
+      <c r="AO1" s="18"/>
+      <c r="AP1" s="18"/>
     </row>
-    <row r="2" spans="1:39" s="8" customFormat="1" ht="12">
+    <row r="2" spans="1:42" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -735,38 +766,41 @@
       <c r="AA2" s="5"/>
       <c r="AB2" s="5"/>
       <c r="AC2" s="5"/>
-      <c r="AD2" s="7">
+      <c r="AD2" s="5"/>
+      <c r="AE2" s="5"/>
+      <c r="AF2" s="5"/>
+      <c r="AG2" s="7">
         <v>1</v>
       </c>
-      <c r="AE2" s="7">
+      <c r="AH2" s="7">
         <v>2</v>
       </c>
-      <c r="AF2" s="7">
+      <c r="AI2" s="7">
         <v>3</v>
       </c>
-      <c r="AG2" s="7">
+      <c r="AJ2" s="7">
         <v>4</v>
       </c>
-      <c r="AH2" s="7">
+      <c r="AK2" s="7">
         <v>5</v>
       </c>
-      <c r="AI2" s="7">
+      <c r="AL2" s="7">
         <v>6</v>
       </c>
-      <c r="AJ2" s="7">
+      <c r="AM2" s="7">
         <v>7</v>
       </c>
-      <c r="AK2" s="7">
+      <c r="AN2" s="7">
         <v>8</v>
       </c>
-      <c r="AL2" s="7">
+      <c r="AO2" s="7">
         <v>9</v>
       </c>
-      <c r="AM2" s="7">
+      <c r="AP2" s="7">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:39" ht="17">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -841,27 +875,27 @@
         <v>11</v>
       </c>
       <c r="Z3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB3" s="3">
+        <v>2</v>
+      </c>
+      <c r="AC3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="AA3" s="3" t="s">
+      <c r="AD3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="AB3" s="3">
+      <c r="AE3" s="3">
         <v>1</v>
       </c>
-      <c r="AC3" s="13">
-        <f>(COUNTIF(AD3:AM3,"○")/10)</f>
+      <c r="AF3" s="13">
+        <f>(COUNTIF(AG3:AP3,"○")/10)</f>
         <v>0.9</v>
       </c>
-      <c r="AD3" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE3" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF3" s="10" t="s">
-        <v>12</v>
-      </c>
       <c r="AG3" s="10" t="s">
         <v>12</v>
       </c>
@@ -871,8 +905,8 @@
       <c r="AI3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AJ3" s="9" t="s">
-        <v>11</v>
+      <c r="AJ3" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AK3" s="10" t="s">
         <v>12</v>
@@ -880,11 +914,20 @@
       <c r="AL3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AM3" s="10" t="s">
+      <c r="AM3" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP3" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:39" ht="17">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.4">
       <c r="C4" s="3">
         <v>2</v>
       </c>
@@ -952,45 +995,51 @@
       <c r="X4" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="AA4" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="AB4" s="3">
         <v>2</v>
       </c>
-      <c r="AC4" s="13">
-        <f t="shared" ref="AC4:AC36" si="1">(COUNTIF(AD4:AM4,"○")/10)</f>
+      <c r="AE4" s="3">
+        <v>2</v>
+      </c>
+      <c r="AF4" s="13">
+        <f t="shared" ref="AF4:AF36" si="1">(COUNTIF(AG4:AP4,"○")/10)</f>
         <v>0.7</v>
       </c>
-      <c r="AD4" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE4" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF4" s="10" t="s">
-        <v>12</v>
-      </c>
       <c r="AG4" s="10" t="s">
         <v>12</v>
       </c>
       <c r="AH4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AI4" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJ4" s="9" t="s">
-        <v>11</v>
+      <c r="AI4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ4" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AK4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AL4" s="10" t="s">
-        <v>12</v>
+      <c r="AL4" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="AM4" s="9" t="s">
         <v>11</v>
       </c>
+      <c r="AN4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP4" s="9" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="5" spans="1:39">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.4">
       <c r="D5" s="13"/>
       <c r="E5" s="11">
         <f>(COUNTIF(E3:E4,"○"))/2</f>
@@ -1072,19 +1121,25 @@
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="AC5" s="13"/>
-      <c r="AD5" s="10"/>
-      <c r="AE5" s="1"/>
-      <c r="AF5" s="1"/>
-      <c r="AG5" s="1"/>
+      <c r="AA5" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF5" s="13"/>
+      <c r="AG5" s="10"/>
       <c r="AH5" s="1"/>
       <c r="AI5" s="1"/>
       <c r="AJ5" s="1"/>
       <c r="AK5" s="1"/>
       <c r="AL5" s="1"/>
       <c r="AM5" s="1"/>
+      <c r="AN5" s="1"/>
+      <c r="AO5" s="1"/>
+      <c r="AP5" s="1"/>
     </row>
-    <row r="6" spans="1:39" ht="17">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.4">
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
@@ -1155,36 +1210,30 @@
       <c r="X6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AA6" s="3" t="s">
+      <c r="AB6" s="3">
         <v>2</v>
       </c>
-      <c r="AB6" s="3">
+      <c r="AD6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="AE6" s="3">
         <v>1</v>
       </c>
-      <c r="AC6" s="13">
+      <c r="AF6" s="13">
         <f t="shared" si="1"/>
         <v>0.7</v>
       </c>
-      <c r="AD6" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE6" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF6" s="10" t="s">
-        <v>12</v>
-      </c>
       <c r="AG6" s="10" t="s">
         <v>12</v>
       </c>
       <c r="AH6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AI6" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AJ6" s="9" t="s">
-        <v>11</v>
+      <c r="AI6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AJ6" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AK6" s="10" t="s">
         <v>12</v>
@@ -1192,11 +1241,20 @@
       <c r="AL6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AM6" s="10" t="s">
+      <c r="AM6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AP6" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:39" ht="17">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.4">
       <c r="C7" s="3">
         <v>2</v>
       </c>
@@ -1264,27 +1322,27 @@
       <c r="X7" s="9" t="s">
         <v>11</v>
       </c>
+      <c r="Z7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA7" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="AB7" s="3">
+        <v>3</v>
+      </c>
+      <c r="AE7" s="3">
         <v>2</v>
       </c>
-      <c r="AC7" s="13">
+      <c r="AF7" s="13">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
-      <c r="AD7" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE7" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF7" s="10" t="s">
-        <v>12</v>
-      </c>
       <c r="AG7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AH7" s="9" t="s">
-        <v>11</v>
+      <c r="AH7" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AI7" s="10" t="s">
         <v>12</v>
@@ -1292,8 +1350,8 @@
       <c r="AJ7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AK7" s="10" t="s">
-        <v>12</v>
+      <c r="AK7" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="AL7" s="10" t="s">
         <v>12</v>
@@ -1301,8 +1359,17 @@
       <c r="AM7" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="AN7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP7" s="10" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="8" spans="1:39" ht="17">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.4">
       <c r="C8" s="3">
         <v>3</v>
       </c>
@@ -1370,22 +1437,19 @@
       <c r="X8" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="AA8" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="AB8" s="3">
+        <v>8</v>
+      </c>
+      <c r="AE8" s="3">
         <v>3</v>
       </c>
-      <c r="AC8" s="13">
+      <c r="AF8" s="13">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
-      <c r="AD8" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE8" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AF8" s="10" t="s">
-        <v>12</v>
-      </c>
       <c r="AG8" s="10" t="s">
         <v>12</v>
       </c>
@@ -1398,8 +1462,8 @@
       <c r="AJ8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AK8" s="10" t="s">
-        <v>12</v>
+      <c r="AK8" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="AL8" s="10" t="s">
         <v>12</v>
@@ -1407,8 +1471,17 @@
       <c r="AM8" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="AN8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP8" s="10" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="9" spans="1:39" ht="17">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.4">
       <c r="C9" s="3">
         <v>4</v>
       </c>
@@ -1476,30 +1549,27 @@
       <c r="X9" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="AA9" t="s">
+        <v>19</v>
+      </c>
       <c r="AB9" s="3">
+        <v>3</v>
+      </c>
+      <c r="AE9" s="3">
         <v>4</v>
       </c>
-      <c r="AC9" s="13">
+      <c r="AF9" s="13">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
-      <c r="AD9" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE9" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF9" s="10" t="s">
-        <v>12</v>
-      </c>
       <c r="AG9" s="10" t="s">
         <v>12</v>
       </c>
       <c r="AH9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AI9" s="9" t="s">
-        <v>11</v>
+      <c r="AI9" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AJ9" s="10" t="s">
         <v>12</v>
@@ -1507,14 +1577,23 @@
       <c r="AK9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AL9" s="10" t="s">
-        <v>12</v>
+      <c r="AL9" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="AM9" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="AN9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP9" s="10" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="10" spans="1:39" ht="17">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.4">
       <c r="C10" s="3">
         <v>5</v>
       </c>
@@ -1585,21 +1664,15 @@
       <c r="AB10" s="3">
         <v>5</v>
       </c>
-      <c r="AC10" s="13">
+      <c r="AE10" s="3">
+        <v>5</v>
+      </c>
+      <c r="AF10" s="13">
         <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
-      <c r="AD10" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AF10" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AG10" s="9" t="s">
-        <v>11</v>
+      <c r="AG10" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AH10" s="9" t="s">
         <v>11</v>
@@ -1610,17 +1683,26 @@
       <c r="AJ10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AK10" s="10" t="s">
-        <v>12</v>
+      <c r="AK10" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="AL10" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AM10" s="10" t="s">
+      <c r="AM10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP10" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:39" ht="17">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.4">
       <c r="C11" s="3">
         <v>6</v>
       </c>
@@ -1688,45 +1770,54 @@
       <c r="X11" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="Z11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA11" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="AB11" s="3">
+        <v>3</v>
+      </c>
+      <c r="AE11" s="3">
         <v>6</v>
       </c>
-      <c r="AC11" s="13">
+      <c r="AF11" s="13">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
-      <c r="AD11" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE11" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF11" s="10" t="s">
-        <v>12</v>
-      </c>
       <c r="AG11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AH11" s="9" t="s">
-        <v>11</v>
+      <c r="AH11" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AI11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AJ11" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AK11" s="10" t="s">
-        <v>12</v>
+      <c r="AJ11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK11" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="AL11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AM11" s="10" t="s">
+      <c r="AM11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP11" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:39" ht="17">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.4">
       <c r="C12" s="3">
         <v>7</v>
       </c>
@@ -1794,45 +1885,51 @@
       <c r="X12" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="AA12" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="AB12" s="3">
+        <v>6</v>
+      </c>
+      <c r="AE12" s="3">
         <v>7</v>
       </c>
-      <c r="AC12" s="13">
+      <c r="AF12" s="13">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
-      <c r="AD12" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE12" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF12" s="10" t="s">
-        <v>12</v>
-      </c>
       <c r="AG12" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AH12" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AI12" s="9" t="s">
-        <v>11</v>
+      <c r="AH12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI12" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AJ12" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AK12" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AL12" s="10" t="s">
-        <v>12</v>
+      <c r="AK12" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL12" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="AM12" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="AN12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP12" s="10" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="13" spans="1:39" ht="17">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.4">
       <c r="C13" s="3">
         <v>8</v>
       </c>
@@ -1900,22 +1997,19 @@
       <c r="X13" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="AA13" t="s">
+        <v>19</v>
+      </c>
       <c r="AB13" s="3">
+        <v>6</v>
+      </c>
+      <c r="AE13" s="3">
         <v>8</v>
       </c>
-      <c r="AC13" s="13">
+      <c r="AF13" s="13">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
-      <c r="AD13" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE13" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF13" s="10" t="s">
-        <v>12</v>
-      </c>
       <c r="AG13" s="10" t="s">
         <v>12</v>
       </c>
@@ -1925,8 +2019,8 @@
       <c r="AI13" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AJ13" s="9" t="s">
-        <v>11</v>
+      <c r="AJ13" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AK13" s="10" t="s">
         <v>12</v>
@@ -1934,11 +2028,20 @@
       <c r="AL13" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AM13" s="10" t="s">
+      <c r="AM13" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN13" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO13" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP13" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:39" ht="17">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.4">
       <c r="C14" s="3">
         <v>9</v>
       </c>
@@ -2007,44 +2110,47 @@
         <v>12</v>
       </c>
       <c r="AB14" s="3">
+        <v>5</v>
+      </c>
+      <c r="AE14" s="3">
         <v>9</v>
       </c>
-      <c r="AC14" s="13">
+      <c r="AF14" s="13">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
-      <c r="AD14" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE14" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF14" s="10" t="s">
-        <v>12</v>
-      </c>
       <c r="AG14" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AH14" s="9" t="s">
-        <v>11</v>
+      <c r="AH14" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AI14" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AJ14" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AK14" s="10" t="s">
-        <v>12</v>
+      <c r="AJ14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK14" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="AL14" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AM14" s="10" t="s">
+      <c r="AM14" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP14" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:39" ht="17">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.4">
       <c r="C15" s="3">
         <v>10</v>
       </c>
@@ -2112,22 +2218,13 @@
       <c r="X15" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AB15" s="3">
+      <c r="AE15" s="3">
         <v>10</v>
       </c>
-      <c r="AC15" s="13">
+      <c r="AF15" s="13">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
-      <c r="AD15" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE15" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF15" s="10" t="s">
-        <v>12</v>
-      </c>
       <c r="AG15" s="10" t="s">
         <v>12</v>
       </c>
@@ -2137,8 +2234,8 @@
       <c r="AI15" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AJ15" s="9" t="s">
-        <v>11</v>
+      <c r="AJ15" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AK15" s="10" t="s">
         <v>12</v>
@@ -2146,11 +2243,20 @@
       <c r="AL15" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AM15" s="10" t="s">
+      <c r="AM15" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN15" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO15" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP15" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:39">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.4">
       <c r="D16" s="13"/>
       <c r="E16" s="11">
         <f>(COUNTIF(E6:E15,"○"))/10</f>
@@ -2232,19 +2338,19 @@
         <f t="shared" si="3"/>
         <v>0.9</v>
       </c>
-      <c r="AC16" s="13"/>
-      <c r="AD16" s="10"/>
-      <c r="AE16" s="1"/>
-      <c r="AF16" s="1"/>
-      <c r="AG16" s="1"/>
+      <c r="AF16" s="13"/>
+      <c r="AG16" s="10"/>
       <c r="AH16" s="1"/>
       <c r="AI16" s="1"/>
       <c r="AJ16" s="1"/>
       <c r="AK16" s="1"/>
       <c r="AL16" s="1"/>
       <c r="AM16" s="1"/>
+      <c r="AN16" s="1"/>
+      <c r="AO16" s="1"/>
+      <c r="AP16" s="1"/>
     </row>
-    <row r="17" spans="2:39" ht="17">
+    <row r="17" spans="2:42" x14ac:dyDescent="0.4">
       <c r="B17" s="3" t="s">
         <v>3</v>
       </c>
@@ -2315,48 +2421,48 @@
       <c r="X17" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AA17" s="3" t="s">
+      <c r="AD17" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AB17" s="3">
+      <c r="AE17" s="3">
         <v>1</v>
       </c>
-      <c r="AC17" s="13">
+      <c r="AF17" s="13">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
-      <c r="AD17" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE17" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF17" s="10" t="s">
-        <v>12</v>
-      </c>
       <c r="AG17" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AH17" s="9" t="s">
-        <v>11</v>
+      <c r="AH17" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AI17" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AJ17" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AK17" s="10" t="s">
-        <v>12</v>
+      <c r="AJ17" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK17" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="AL17" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AM17" s="10" t="s">
+      <c r="AM17" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN17" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO17" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP17" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="2:39" ht="17">
+    <row r="18" spans="2:42" x14ac:dyDescent="0.4">
       <c r="C18" s="3">
         <v>2</v>
       </c>
@@ -2424,22 +2530,13 @@
       <c r="X18" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AB18" s="3">
+      <c r="AE18" s="3">
         <v>2</v>
       </c>
-      <c r="AC18" s="13">
+      <c r="AF18" s="13">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="AD18" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE18" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF18" s="10" t="s">
-        <v>12</v>
-      </c>
       <c r="AG18" s="10" t="s">
         <v>12</v>
       </c>
@@ -2461,8 +2558,17 @@
       <c r="AM18" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="AN18" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO18" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP18" s="10" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="19" spans="2:39" ht="17">
+    <row r="19" spans="2:42" x14ac:dyDescent="0.4">
       <c r="C19" s="3">
         <v>3</v>
       </c>
@@ -2530,36 +2636,27 @@
       <c r="X19" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AB19" s="3">
+      <c r="AE19" s="3">
         <v>3</v>
       </c>
-      <c r="AC19" s="13">
+      <c r="AF19" s="13">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
-      <c r="AD19" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE19" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF19" s="9" t="s">
-        <v>11</v>
-      </c>
       <c r="AG19" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AH19" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AI19" s="10" t="s">
-        <v>12</v>
+      <c r="AH19" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI19" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="AJ19" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AK19" s="10" t="s">
-        <v>12</v>
+      <c r="AK19" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="AL19" s="10" t="s">
         <v>12</v>
@@ -2567,8 +2664,17 @@
       <c r="AM19" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="AN19" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO19" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP19" s="10" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="20" spans="2:39" ht="17">
+    <row r="20" spans="2:42" x14ac:dyDescent="0.4">
       <c r="C20" s="3">
         <v>4</v>
       </c>
@@ -2636,22 +2742,13 @@
       <c r="X20" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AB20" s="3">
+      <c r="AE20" s="3">
         <v>4</v>
       </c>
-      <c r="AC20" s="13">
+      <c r="AF20" s="13">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
-      <c r="AD20" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE20" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF20" s="10" t="s">
-        <v>12</v>
-      </c>
       <c r="AG20" s="10" t="s">
         <v>12</v>
       </c>
@@ -2661,8 +2758,8 @@
       <c r="AI20" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AJ20" s="9" t="s">
-        <v>11</v>
+      <c r="AJ20" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AK20" s="10" t="s">
         <v>12</v>
@@ -2670,11 +2767,20 @@
       <c r="AL20" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AM20" s="10" t="s">
+      <c r="AM20" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN20" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO20" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP20" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="2:39" ht="17">
+    <row r="21" spans="2:42" x14ac:dyDescent="0.4">
       <c r="C21" s="3">
         <v>5</v>
       </c>
@@ -2742,27 +2848,18 @@
       <c r="X21" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AB21" s="3">
+      <c r="AE21" s="3">
         <v>5</v>
       </c>
-      <c r="AC21" s="13">
+      <c r="AF21" s="13">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
-      <c r="AD21" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE21" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF21" s="10" t="s">
-        <v>12</v>
-      </c>
       <c r="AG21" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AH21" s="9" t="s">
-        <v>11</v>
+      <c r="AH21" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AI21" s="10" t="s">
         <v>12</v>
@@ -2770,8 +2867,8 @@
       <c r="AJ21" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AK21" s="10" t="s">
-        <v>12</v>
+      <c r="AK21" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="AL21" s="10" t="s">
         <v>12</v>
@@ -2779,8 +2876,17 @@
       <c r="AM21" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="AN21" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO21" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP21" s="10" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="22" spans="2:39" ht="17">
+    <row r="22" spans="2:42" x14ac:dyDescent="0.4">
       <c r="C22" s="3">
         <v>6</v>
       </c>
@@ -2848,27 +2954,18 @@
       <c r="X22" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AB22" s="3">
+      <c r="AE22" s="3">
         <v>6</v>
       </c>
-      <c r="AC22" s="13">
+      <c r="AF22" s="13">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
-      <c r="AD22" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE22" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF22" s="10" t="s">
-        <v>12</v>
-      </c>
       <c r="AG22" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AH22" s="9" t="s">
-        <v>11</v>
+      <c r="AH22" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AI22" s="10" t="s">
         <v>12</v>
@@ -2876,8 +2973,8 @@
       <c r="AJ22" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AK22" s="10" t="s">
-        <v>12</v>
+      <c r="AK22" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="AL22" s="10" t="s">
         <v>12</v>
@@ -2885,8 +2982,17 @@
       <c r="AM22" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="AN22" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO22" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP22" s="10" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="23" spans="2:39" ht="17">
+    <row r="23" spans="2:42" x14ac:dyDescent="0.4">
       <c r="C23" s="3">
         <v>7</v>
       </c>
@@ -2954,22 +3060,13 @@
       <c r="X23" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AB23" s="3">
+      <c r="AE23" s="3">
         <v>7</v>
       </c>
-      <c r="AC23" s="13">
+      <c r="AF23" s="13">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="AD23" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE23" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF23" s="10" t="s">
-        <v>12</v>
-      </c>
       <c r="AG23" s="10" t="s">
         <v>12</v>
       </c>
@@ -2991,8 +3088,17 @@
       <c r="AM23" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="AN23" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO23" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP23" s="10" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="24" spans="2:39" ht="17">
+    <row r="24" spans="2:42" x14ac:dyDescent="0.4">
       <c r="C24" s="3">
         <v>8</v>
       </c>
@@ -3060,22 +3166,13 @@
       <c r="X24" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AB24" s="3">
+      <c r="AE24" s="3">
         <v>8</v>
       </c>
-      <c r="AC24" s="13">
+      <c r="AF24" s="13">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="AD24" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE24" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF24" s="10" t="s">
-        <v>12</v>
-      </c>
       <c r="AG24" s="10" t="s">
         <v>12</v>
       </c>
@@ -3097,8 +3194,17 @@
       <c r="AM24" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="AN24" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO24" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP24" s="10" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="25" spans="2:39" ht="17">
+    <row r="25" spans="2:42" x14ac:dyDescent="0.4">
       <c r="C25" s="3">
         <v>9</v>
       </c>
@@ -3166,22 +3272,13 @@
       <c r="X25" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AB25" s="3">
+      <c r="AE25" s="3">
         <v>9</v>
       </c>
-      <c r="AC25" s="13">
+      <c r="AF25" s="13">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
-      <c r="AD25" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE25" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF25" s="10" t="s">
-        <v>12</v>
-      </c>
       <c r="AG25" s="10" t="s">
         <v>12</v>
       </c>
@@ -3191,8 +3288,8 @@
       <c r="AI25" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AJ25" s="9" t="s">
-        <v>11</v>
+      <c r="AJ25" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AK25" s="10" t="s">
         <v>12</v>
@@ -3200,11 +3297,20 @@
       <c r="AL25" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AM25" s="10" t="s">
+      <c r="AM25" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN25" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO25" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP25" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="2:39" ht="17">
+    <row r="26" spans="2:42" x14ac:dyDescent="0.4">
       <c r="C26" s="3">
         <v>10</v>
       </c>
@@ -3272,30 +3378,21 @@
       <c r="X26" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AB26" s="3">
+      <c r="AE26" s="3">
         <v>10</v>
       </c>
-      <c r="AC26" s="13">
+      <c r="AF26" s="13">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
-      <c r="AD26" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE26" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF26" s="9" t="s">
-        <v>11</v>
-      </c>
       <c r="AG26" s="10" t="s">
         <v>12</v>
       </c>
       <c r="AH26" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AI26" s="10" t="s">
-        <v>12</v>
+      <c r="AI26" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="AJ26" s="10" t="s">
         <v>12</v>
@@ -3309,8 +3406,17 @@
       <c r="AM26" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="AN26" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO26" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP26" s="10" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="27" spans="2:39" ht="17">
+    <row r="27" spans="2:42" x14ac:dyDescent="0.4">
       <c r="C27" s="3">
         <v>11</v>
       </c>
@@ -3378,22 +3484,13 @@
       <c r="X27" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AB27" s="3">
-        <v>11</v>
-      </c>
-      <c r="AC27" s="13">
+      <c r="AE27" s="3">
+        <v>11</v>
+      </c>
+      <c r="AF27" s="13">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="AD27" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE27" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF27" s="10" t="s">
-        <v>12</v>
-      </c>
       <c r="AG27" s="10" t="s">
         <v>12</v>
       </c>
@@ -3415,8 +3512,17 @@
       <c r="AM27" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="AN27" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO27" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP27" s="10" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="28" spans="2:39" ht="17">
+    <row r="28" spans="2:42" x14ac:dyDescent="0.4">
       <c r="C28" s="3">
         <v>12</v>
       </c>
@@ -3484,22 +3590,13 @@
       <c r="X28" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AB28" s="3">
-        <v>12</v>
-      </c>
-      <c r="AC28" s="13">
+      <c r="AE28" s="3">
+        <v>12</v>
+      </c>
+      <c r="AF28" s="13">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="AD28" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE28" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF28" s="10" t="s">
-        <v>12</v>
-      </c>
       <c r="AG28" s="10" t="s">
         <v>12</v>
       </c>
@@ -3521,8 +3618,17 @@
       <c r="AM28" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="AN28" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO28" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP28" s="10" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="29" spans="2:39" ht="17">
+    <row r="29" spans="2:42" x14ac:dyDescent="0.4">
       <c r="C29" s="3">
         <v>13</v>
       </c>
@@ -3590,45 +3696,45 @@
       <c r="X29" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AB29" s="3">
+      <c r="AE29" s="3">
         <v>13</v>
       </c>
-      <c r="AC29" s="13">
+      <c r="AF29" s="13">
         <f t="shared" si="1"/>
         <v>0.7</v>
       </c>
-      <c r="AD29" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE29" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF29" s="10" t="s">
-        <v>12</v>
-      </c>
       <c r="AG29" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AH29" s="9" t="s">
-        <v>11</v>
+      <c r="AH29" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AI29" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AJ29" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AK29" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AL29" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AM29" s="10" t="s">
+      <c r="AJ29" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AK29" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL29" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM29" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN29" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO29" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AP29" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="2:39" ht="17">
+    <row r="30" spans="2:42" x14ac:dyDescent="0.4">
       <c r="C30" s="3">
         <v>14</v>
       </c>
@@ -3696,27 +3802,18 @@
       <c r="X30" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AB30" s="3">
+      <c r="AE30" s="3">
         <v>14</v>
       </c>
-      <c r="AC30" s="13">
+      <c r="AF30" s="13">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
-      <c r="AD30" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE30" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF30" s="10" t="s">
-        <v>12</v>
-      </c>
       <c r="AG30" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AH30" s="9" t="s">
-        <v>11</v>
+      <c r="AH30" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AI30" s="10" t="s">
         <v>12</v>
@@ -3724,8 +3821,8 @@
       <c r="AJ30" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AK30" s="10" t="s">
-        <v>12</v>
+      <c r="AK30" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="AL30" s="10" t="s">
         <v>12</v>
@@ -3733,8 +3830,17 @@
       <c r="AM30" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="AN30" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO30" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP30" s="10" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="31" spans="2:39" ht="17">
+    <row r="31" spans="2:42" x14ac:dyDescent="0.4">
       <c r="D31" s="5"/>
       <c r="E31" s="16">
         <f>(COUNTIF(E17:E30,"○"))/14</f>
@@ -3816,25 +3922,16 @@
         <f t="shared" si="4"/>
         <v>7.1428571428571425E-2</v>
       </c>
-      <c r="AA31" s="3" t="s">
+      <c r="AD31" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="AB31" s="3">
+      <c r="AE31" s="3">
         <v>1</v>
       </c>
-      <c r="AC31" s="13">
+      <c r="AF31" s="13">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
-      <c r="AD31" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE31" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF31" s="10" t="s">
-        <v>12</v>
-      </c>
       <c r="AG31" s="10" t="s">
         <v>12</v>
       </c>
@@ -3844,8 +3941,8 @@
       <c r="AI31" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AJ31" s="9" t="s">
-        <v>11</v>
+      <c r="AJ31" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AK31" s="10" t="s">
         <v>12</v>
@@ -3853,32 +3950,32 @@
       <c r="AL31" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AM31" s="10" t="s">
+      <c r="AM31" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN31" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO31" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP31" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="2:39" ht="17">
-      <c r="AB32" s="3">
+    <row r="32" spans="2:42" x14ac:dyDescent="0.4">
+      <c r="AE32" s="3">
         <v>2</v>
       </c>
-      <c r="AC32" s="13">
+      <c r="AF32" s="13">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
-      <c r="AD32" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE32" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF32" s="10" t="s">
-        <v>12</v>
-      </c>
       <c r="AG32" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AH32" s="9" t="s">
-        <v>11</v>
+      <c r="AH32" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AI32" s="10" t="s">
         <v>12</v>
@@ -3886,36 +3983,36 @@
       <c r="AJ32" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AK32" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AL32" s="9" t="s">
-        <v>11</v>
+      <c r="AK32" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AL32" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AM32" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="AN32" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO32" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AP32" s="10" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="33" spans="27:39">
-      <c r="AA33" s="3" t="s">
+    <row r="33" spans="30:42" x14ac:dyDescent="0.4">
+      <c r="AD33" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="AB33" s="3">
+      <c r="AE33" s="3">
         <v>1</v>
       </c>
-      <c r="AC33" s="13">
+      <c r="AF33" s="13">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="AD33" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE33" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF33" s="10" t="s">
-        <v>12</v>
-      </c>
       <c r="AG33" s="10" t="s">
         <v>12</v>
       </c>
@@ -3937,24 +4034,24 @@
       <c r="AM33" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="AN33" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO33" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP33" s="10" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="34" spans="27:39" ht="17">
-      <c r="AB34" s="3">
+    <row r="34" spans="30:42" x14ac:dyDescent="0.4">
+      <c r="AE34" s="3">
         <v>2</v>
       </c>
-      <c r="AC34" s="13">
+      <c r="AF34" s="13">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
-      <c r="AD34" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE34" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF34" s="10" t="s">
-        <v>12</v>
-      </c>
       <c r="AG34" s="10" t="s">
         <v>12</v>
       </c>
@@ -3964,8 +4061,8 @@
       <c r="AI34" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AJ34" s="9" t="s">
-        <v>11</v>
+      <c r="AJ34" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AK34" s="10" t="s">
         <v>12</v>
@@ -3973,27 +4070,27 @@
       <c r="AL34" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AM34" s="10" t="s">
+      <c r="AM34" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AN34" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO34" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP34" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="27:39" ht="17">
-      <c r="AB35" s="3">
+    <row r="35" spans="30:42" x14ac:dyDescent="0.4">
+      <c r="AE35" s="3">
         <v>3</v>
       </c>
-      <c r="AC35" s="13">
+      <c r="AF35" s="13">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
-      <c r="AD35" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE35" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF35" s="10" t="s">
-        <v>12</v>
-      </c>
       <c r="AG35" s="10" t="s">
         <v>12</v>
       </c>
@@ -4009,33 +4106,33 @@
       <c r="AK35" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AL35" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AM35" s="9" t="s">
+      <c r="AL35" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AM35" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AN35" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO35" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AP35" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="27:39">
-      <c r="AA36" s="3" t="s">
+    <row r="36" spans="30:42" x14ac:dyDescent="0.4">
+      <c r="AD36" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="AB36" s="3">
+      <c r="AE36" s="3">
         <v>1</v>
       </c>
-      <c r="AC36" s="13">
+      <c r="AF36" s="13">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="AD36" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AE36" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AF36" s="10" t="s">
-        <v>12</v>
-      </c>
       <c r="AG36" s="10" t="s">
         <v>12</v>
       </c>
@@ -4057,45 +4154,54 @@
       <c r="AM36" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="AN36" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AO36" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AP36" s="10" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="37" spans="27:39">
-      <c r="AD37" s="16">
-        <f>(COUNTIF(AD3:AD36,"○")/32)</f>
+    <row r="37" spans="30:42" x14ac:dyDescent="0.4">
+      <c r="AG37" s="16">
+        <f>(COUNTIF(AG3:AG36,"○")/32)</f>
         <v>1</v>
       </c>
-      <c r="AE37" s="16">
-        <f t="shared" ref="AE37:AM37" si="5">(COUNTIF(AE3:AE36,"○")/32)</f>
+      <c r="AH37" s="16">
+        <f t="shared" ref="AH37:AP37" si="5">(COUNTIF(AH3:AH36,"○")/32)</f>
         <v>0.9375</v>
       </c>
-      <c r="AF37" s="16">
+      <c r="AI37" s="16">
         <f t="shared" si="5"/>
         <v>0.9375</v>
       </c>
-      <c r="AG37" s="16">
+      <c r="AJ37" s="16">
         <f t="shared" si="5"/>
         <v>0.96875</v>
       </c>
-      <c r="AH37" s="16">
+      <c r="AK37" s="16">
         <f t="shared" si="5"/>
         <v>0.59375</v>
-      </c>
-      <c r="AI37" s="16">
-        <f t="shared" si="5"/>
-        <v>0.875</v>
-      </c>
-      <c r="AJ37" s="16">
-        <f t="shared" si="5"/>
-        <v>0.5625</v>
-      </c>
-      <c r="AK37" s="16">
-        <f t="shared" si="5"/>
-        <v>1</v>
       </c>
       <c r="AL37" s="16">
         <f t="shared" si="5"/>
         <v>0.875</v>
       </c>
       <c r="AM37" s="16">
+        <f t="shared" si="5"/>
+        <v>0.5625</v>
+      </c>
+      <c r="AN37" s="16">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="AO37" s="16">
+        <f t="shared" si="5"/>
+        <v>0.875</v>
+      </c>
+      <c r="AP37" s="16">
         <f t="shared" si="5"/>
         <v>0.9375</v>
       </c>
@@ -4103,7 +4209,7 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="E1:X1"/>
-    <mergeCell ref="AD1:AM1"/>
+    <mergeCell ref="AG1:AP1"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[add] added analyze files
</commit_message>
<xml_diff>
--- a/Answer-Data.xlsx
+++ b/Answer-Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC_User\iCloudDrive\Documents\01_University\02_Research\Working-Directory\eye-tracking-software\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D201D5D8-219D-4C77-84C5-7AFDCBA3E483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3248773E-4072-4592-86B1-CF84B09D554D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{65F65776-174E-4145-8CCF-AA6B8A50F68A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="16">
   <si>
     <t>English</t>
   </si>
@@ -115,34 +115,6 @@
     <rPh sb="0" eb="2">
       <t>カイトウ</t>
     </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>J1</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>elbow</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>BIC</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>Silhouette</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>J2</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>J3</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>-</t>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -613,26 +585,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60C853D4-11AD-448C-900A-323815755F36}">
-  <dimension ref="A1:AP37"/>
+  <dimension ref="A1:AM37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AB15" sqref="AB15"/>
+      <selection activeCell="AB9" sqref="AB9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="10" style="3" customWidth="1"/>
     <col min="2" max="3" width="4.125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="6.125" style="14" customWidth="1"/>
+    <col min="4" max="4" width="6.25" style="14" customWidth="1"/>
     <col min="5" max="24" width="4.375" style="2" customWidth="1"/>
     <col min="25" max="25" width="4.125" style="3" customWidth="1"/>
-    <col min="26" max="29" width="10" style="3" customWidth="1"/>
-    <col min="30" max="31" width="4.125" style="3" customWidth="1"/>
-    <col min="32" max="32" width="6.125" style="3" customWidth="1"/>
-    <col min="33" max="42" width="4.375" style="4" customWidth="1"/>
+    <col min="26" max="26" width="10" style="3" customWidth="1"/>
+    <col min="27" max="28" width="4.125" style="3" customWidth="1"/>
+    <col min="29" max="29" width="6.125" style="3" customWidth="1"/>
+    <col min="30" max="39" width="4.375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" s="8" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:39" s="8" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>10</v>
       </c>
@@ -668,35 +640,32 @@
       <c r="W1" s="17"/>
       <c r="X1" s="17"/>
       <c r="Y1" s="5"/>
-      <c r="Z1" s="5"/>
-      <c r="AA1" s="5"/>
-      <c r="AB1" s="5"/>
-      <c r="AC1" s="5" t="s">
+      <c r="Z1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="AD1" s="5" t="s">
+      <c r="AA1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="AE1" s="5" t="s">
+      <c r="AB1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="AF1" s="15" t="s">
+      <c r="AC1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="AG1" s="18" t="s">
+      <c r="AD1" s="18" t="s">
         <v>15</v>
       </c>
+      <c r="AE1" s="18"/>
+      <c r="AF1" s="18"/>
+      <c r="AG1" s="18"/>
       <c r="AH1" s="18"/>
       <c r="AI1" s="18"/>
       <c r="AJ1" s="18"/>
       <c r="AK1" s="18"/>
       <c r="AL1" s="18"/>
       <c r="AM1" s="18"/>
-      <c r="AN1" s="18"/>
-      <c r="AO1" s="18"/>
-      <c r="AP1" s="18"/>
     </row>
-    <row r="2" spans="1:42" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:39" s="8" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -766,41 +735,38 @@
       <c r="AA2" s="5"/>
       <c r="AB2" s="5"/>
       <c r="AC2" s="5"/>
-      <c r="AD2" s="5"/>
-      <c r="AE2" s="5"/>
-      <c r="AF2" s="5"/>
+      <c r="AD2" s="7">
+        <v>1</v>
+      </c>
+      <c r="AE2" s="7">
+        <v>2</v>
+      </c>
+      <c r="AF2" s="7">
+        <v>3</v>
+      </c>
       <c r="AG2" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AH2" s="7">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AI2" s="7">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AJ2" s="7">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="AK2" s="7">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="AL2" s="7">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="AM2" s="7">
-        <v>7</v>
-      </c>
-      <c r="AN2" s="7">
-        <v>8</v>
-      </c>
-      <c r="AO2" s="7">
-        <v>9</v>
-      </c>
-      <c r="AP2" s="7">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -875,27 +841,27 @@
         <v>11</v>
       </c>
       <c r="Z3" s="3" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="AA3" s="3" t="s">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="AB3" s="3">
-        <v>2</v>
-      </c>
-      <c r="AC3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="AD3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="AE3" s="3">
-        <v>1</v>
-      </c>
-      <c r="AF3" s="13">
-        <f>(COUNTIF(AG3:AP3,"○")/10)</f>
+      <c r="AC3" s="13">
+        <f>(COUNTIF(AD3:AM3,"○")/10)</f>
         <v>0.9</v>
       </c>
+      <c r="AD3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF3" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AG3" s="10" t="s">
         <v>12</v>
       </c>
@@ -905,8 +871,8 @@
       <c r="AI3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AJ3" s="10" t="s">
-        <v>12</v>
+      <c r="AJ3" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="AK3" s="10" t="s">
         <v>12</v>
@@ -914,20 +880,11 @@
       <c r="AL3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AM3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AN3" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AO3" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AP3" s="10" t="s">
+      <c r="AM3" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.4">
       <c r="C4" s="3">
         <v>2</v>
       </c>
@@ -995,51 +952,45 @@
       <c r="X4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AA4" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="AB4" s="3">
         <v>2</v>
       </c>
-      <c r="AE4" s="3">
-        <v>2</v>
-      </c>
-      <c r="AF4" s="13">
-        <f t="shared" ref="AF4:AF36" si="1">(COUNTIF(AG4:AP4,"○")/10)</f>
+      <c r="AC4" s="13">
+        <f t="shared" ref="AC4:AC36" si="1">(COUNTIF(AD4:AM4,"○")/10)</f>
         <v>0.7</v>
       </c>
+      <c r="AD4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE4" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF4" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AG4" s="10" t="s">
         <v>12</v>
       </c>
       <c r="AH4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AI4" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AJ4" s="10" t="s">
-        <v>12</v>
+      <c r="AI4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ4" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="AK4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AL4" s="9" t="s">
-        <v>11</v>
+      <c r="AL4" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AM4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AN4" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AO4" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AP4" s="9" t="s">
-        <v>11</v>
-      </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.4">
       <c r="D5" s="13"/>
       <c r="E5" s="11">
         <f>(COUNTIF(E3:E4,"○"))/2</f>
@@ -1121,25 +1072,19 @@
         <f t="shared" si="2"/>
         <v>0.5</v>
       </c>
-      <c r="AA5" t="s">
-        <v>19</v>
-      </c>
-      <c r="AB5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF5" s="13"/>
-      <c r="AG5" s="10"/>
+      <c r="AC5" s="13"/>
+      <c r="AD5" s="10"/>
+      <c r="AE5" s="1"/>
+      <c r="AF5" s="1"/>
+      <c r="AG5" s="1"/>
       <c r="AH5" s="1"/>
       <c r="AI5" s="1"/>
       <c r="AJ5" s="1"/>
       <c r="AK5" s="1"/>
       <c r="AL5" s="1"/>
       <c r="AM5" s="1"/>
-      <c r="AN5" s="1"/>
-      <c r="AO5" s="1"/>
-      <c r="AP5" s="1"/>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.4">
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
@@ -1210,30 +1155,36 @@
       <c r="X6" s="10" t="s">
         <v>12</v>
       </c>
+      <c r="AA6" s="3" t="s">
+        <v>2</v>
+      </c>
       <c r="AB6" s="3">
-        <v>2</v>
-      </c>
-      <c r="AD6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE6" s="3">
         <v>1</v>
       </c>
-      <c r="AF6" s="13">
+      <c r="AC6" s="13">
         <f t="shared" si="1"/>
         <v>0.7</v>
       </c>
+      <c r="AD6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE6" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF6" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AG6" s="10" t="s">
         <v>12</v>
       </c>
       <c r="AH6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AI6" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AJ6" s="10" t="s">
-        <v>12</v>
+      <c r="AI6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AJ6" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="AK6" s="10" t="s">
         <v>12</v>
@@ -1241,20 +1192,11 @@
       <c r="AL6" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AM6" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AN6" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AO6" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AP6" s="10" t="s">
+      <c r="AM6" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.4">
       <c r="C7" s="3">
         <v>2</v>
       </c>
@@ -1322,27 +1264,27 @@
       <c r="X7" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="Z7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA7" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="AB7" s="3">
-        <v>3</v>
-      </c>
-      <c r="AE7" s="3">
         <v>2</v>
       </c>
-      <c r="AF7" s="13">
+      <c r="AC7" s="13">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
+      <c r="AD7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF7" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AG7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AH7" s="10" t="s">
-        <v>12</v>
+      <c r="AH7" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="AI7" s="10" t="s">
         <v>12</v>
@@ -1350,8 +1292,8 @@
       <c r="AJ7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AK7" s="9" t="s">
-        <v>11</v>
+      <c r="AK7" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AL7" s="10" t="s">
         <v>12</v>
@@ -1359,17 +1301,8 @@
       <c r="AM7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AN7" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AO7" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AP7" s="10" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.4">
       <c r="C8" s="3">
         <v>3</v>
       </c>
@@ -1437,19 +1370,22 @@
       <c r="X8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AA8" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="AB8" s="3">
-        <v>8</v>
-      </c>
-      <c r="AE8" s="3">
         <v>3</v>
       </c>
-      <c r="AF8" s="13">
+      <c r="AC8" s="13">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
+      <c r="AD8" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF8" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AG8" s="10" t="s">
         <v>12</v>
       </c>
@@ -1462,8 +1398,8 @@
       <c r="AJ8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AK8" s="9" t="s">
-        <v>11</v>
+      <c r="AK8" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AL8" s="10" t="s">
         <v>12</v>
@@ -1471,17 +1407,8 @@
       <c r="AM8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AN8" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AO8" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AP8" s="10" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.4">
       <c r="C9" s="3">
         <v>4</v>
       </c>
@@ -1549,27 +1476,30 @@
       <c r="X9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AA9" t="s">
-        <v>19</v>
-      </c>
       <c r="AB9" s="3">
-        <v>3</v>
-      </c>
-      <c r="AE9" s="3">
         <v>4</v>
       </c>
-      <c r="AF9" s="13">
+      <c r="AC9" s="13">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
+      <c r="AD9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE9" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF9" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AG9" s="10" t="s">
         <v>12</v>
       </c>
       <c r="AH9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AI9" s="10" t="s">
-        <v>12</v>
+      <c r="AI9" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="AJ9" s="10" t="s">
         <v>12</v>
@@ -1577,23 +1507,14 @@
       <c r="AK9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AL9" s="9" t="s">
-        <v>11</v>
+      <c r="AL9" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AM9" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AN9" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AO9" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AP9" s="10" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.4">
       <c r="C10" s="3">
         <v>5</v>
       </c>
@@ -1664,15 +1585,21 @@
       <c r="AB10" s="3">
         <v>5</v>
       </c>
-      <c r="AE10" s="3">
-        <v>5</v>
-      </c>
-      <c r="AF10" s="13">
+      <c r="AC10" s="13">
         <f t="shared" si="1"/>
         <v>0.6</v>
       </c>
-      <c r="AG10" s="10" t="s">
-        <v>12</v>
+      <c r="AD10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF10" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AG10" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="AH10" s="9" t="s">
         <v>11</v>
@@ -1683,26 +1610,17 @@
       <c r="AJ10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AK10" s="9" t="s">
-        <v>11</v>
+      <c r="AK10" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AL10" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AM10" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AN10" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AO10" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AP10" s="10" t="s">
+      <c r="AM10" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.4">
       <c r="C11" s="3">
         <v>6</v>
       </c>
@@ -1770,54 +1688,45 @@
       <c r="X11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="Z11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="AA11" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="AB11" s="3">
-        <v>3</v>
-      </c>
-      <c r="AE11" s="3">
         <v>6</v>
       </c>
-      <c r="AF11" s="13">
+      <c r="AC11" s="13">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
+      <c r="AD11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF11" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AG11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AH11" s="10" t="s">
-        <v>12</v>
+      <c r="AH11" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="AI11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AJ11" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AK11" s="9" t="s">
-        <v>11</v>
+      <c r="AJ11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AK11" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AL11" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AM11" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AN11" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AO11" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AP11" s="10" t="s">
+      <c r="AM11" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.4">
       <c r="C12" s="3">
         <v>7</v>
       </c>
@@ -1885,51 +1794,45 @@
       <c r="X12" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AA12" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="AB12" s="3">
-        <v>6</v>
-      </c>
-      <c r="AE12" s="3">
         <v>7</v>
       </c>
-      <c r="AF12" s="13">
+      <c r="AC12" s="13">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
+      <c r="AD12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF12" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AG12" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AH12" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AI12" s="10" t="s">
-        <v>12</v>
+      <c r="AH12" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AI12" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="AJ12" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AK12" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AL12" s="9" t="s">
-        <v>11</v>
+      <c r="AK12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL12" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AM12" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AN12" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AO12" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AP12" s="10" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.4">
       <c r="C13" s="3">
         <v>8</v>
       </c>
@@ -1997,19 +1900,22 @@
       <c r="X13" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AA13" t="s">
-        <v>19</v>
-      </c>
       <c r="AB13" s="3">
-        <v>6</v>
-      </c>
-      <c r="AE13" s="3">
         <v>8</v>
       </c>
-      <c r="AF13" s="13">
+      <c r="AC13" s="13">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
+      <c r="AD13" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE13" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF13" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AG13" s="10" t="s">
         <v>12</v>
       </c>
@@ -2019,8 +1925,8 @@
       <c r="AI13" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AJ13" s="10" t="s">
-        <v>12</v>
+      <c r="AJ13" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="AK13" s="10" t="s">
         <v>12</v>
@@ -2028,20 +1934,11 @@
       <c r="AL13" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AM13" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AN13" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AO13" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AP13" s="10" t="s">
+      <c r="AM13" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:39" x14ac:dyDescent="0.4">
       <c r="C14" s="3">
         <v>9</v>
       </c>
@@ -2110,47 +2007,44 @@
         <v>12</v>
       </c>
       <c r="AB14" s="3">
-        <v>5</v>
-      </c>
-      <c r="AE14" s="3">
         <v>9</v>
       </c>
-      <c r="AF14" s="13">
+      <c r="AC14" s="13">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
+      <c r="AD14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE14" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF14" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AG14" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AH14" s="10" t="s">
-        <v>12</v>
+      <c r="AH14" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="AI14" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AJ14" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AK14" s="9" t="s">
-        <v>11</v>
+      <c r="AJ14" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AK14" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AL14" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AM14" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AN14" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AO14" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AP14" s="10" t="s">
+      <c r="AM14" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.4">
       <c r="C15" s="3">
         <v>10</v>
       </c>
@@ -2218,13 +2112,22 @@
       <c r="X15" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AE15" s="3">
+      <c r="AB15" s="3">
         <v>10</v>
       </c>
-      <c r="AF15" s="13">
+      <c r="AC15" s="13">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
+      <c r="AD15" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE15" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF15" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AG15" s="10" t="s">
         <v>12</v>
       </c>
@@ -2234,8 +2137,8 @@
       <c r="AI15" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AJ15" s="10" t="s">
-        <v>12</v>
+      <c r="AJ15" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="AK15" s="10" t="s">
         <v>12</v>
@@ -2243,20 +2146,11 @@
       <c r="AL15" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AM15" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AN15" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AO15" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AP15" s="10" t="s">
+      <c r="AM15" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.4">
       <c r="D16" s="13"/>
       <c r="E16" s="11">
         <f>(COUNTIF(E6:E15,"○"))/10</f>
@@ -2338,19 +2232,19 @@
         <f t="shared" si="3"/>
         <v>0.9</v>
       </c>
-      <c r="AF16" s="13"/>
-      <c r="AG16" s="10"/>
+      <c r="AC16" s="13"/>
+      <c r="AD16" s="10"/>
+      <c r="AE16" s="1"/>
+      <c r="AF16" s="1"/>
+      <c r="AG16" s="1"/>
       <c r="AH16" s="1"/>
       <c r="AI16" s="1"/>
       <c r="AJ16" s="1"/>
       <c r="AK16" s="1"/>
       <c r="AL16" s="1"/>
       <c r="AM16" s="1"/>
-      <c r="AN16" s="1"/>
-      <c r="AO16" s="1"/>
-      <c r="AP16" s="1"/>
     </row>
-    <row r="17" spans="2:42" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:39" x14ac:dyDescent="0.4">
       <c r="B17" s="3" t="s">
         <v>3</v>
       </c>
@@ -2421,48 +2315,48 @@
       <c r="X17" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AD17" s="3" t="s">
+      <c r="AA17" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="AE17" s="3">
+      <c r="AB17" s="3">
         <v>1</v>
       </c>
-      <c r="AF17" s="13">
+      <c r="AC17" s="13">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
+      <c r="AD17" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE17" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF17" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AG17" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AH17" s="10" t="s">
-        <v>12</v>
+      <c r="AH17" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="AI17" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AJ17" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AK17" s="9" t="s">
-        <v>11</v>
+      <c r="AJ17" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AK17" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AL17" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AM17" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AN17" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AO17" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AP17" s="10" t="s">
+      <c r="AM17" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="2:42" x14ac:dyDescent="0.4">
+    <row r="18" spans="2:39" x14ac:dyDescent="0.4">
       <c r="C18" s="3">
         <v>2</v>
       </c>
@@ -2530,13 +2424,22 @@
       <c r="X18" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AE18" s="3">
+      <c r="AB18" s="3">
         <v>2</v>
       </c>
-      <c r="AF18" s="13">
+      <c r="AC18" s="13">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
+      <c r="AD18" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE18" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF18" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AG18" s="10" t="s">
         <v>12</v>
       </c>
@@ -2558,17 +2461,8 @@
       <c r="AM18" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AN18" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AO18" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AP18" s="10" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="19" spans="2:42" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:39" x14ac:dyDescent="0.4">
       <c r="C19" s="3">
         <v>3</v>
       </c>
@@ -2636,27 +2530,36 @@
       <c r="X19" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AE19" s="3">
+      <c r="AB19" s="3">
         <v>3</v>
       </c>
-      <c r="AF19" s="13">
+      <c r="AC19" s="13">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
+      <c r="AD19" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE19" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF19" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="AG19" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AH19" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AI19" s="9" t="s">
-        <v>11</v>
+      <c r="AH19" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AI19" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AJ19" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AK19" s="9" t="s">
-        <v>11</v>
+      <c r="AK19" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AL19" s="10" t="s">
         <v>12</v>
@@ -2664,17 +2567,8 @@
       <c r="AM19" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AN19" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AO19" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AP19" s="10" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="20" spans="2:42" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:39" x14ac:dyDescent="0.4">
       <c r="C20" s="3">
         <v>4</v>
       </c>
@@ -2742,13 +2636,22 @@
       <c r="X20" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AE20" s="3">
+      <c r="AB20" s="3">
         <v>4</v>
       </c>
-      <c r="AF20" s="13">
+      <c r="AC20" s="13">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
+      <c r="AD20" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE20" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF20" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AG20" s="10" t="s">
         <v>12</v>
       </c>
@@ -2758,8 +2661,8 @@
       <c r="AI20" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AJ20" s="10" t="s">
-        <v>12</v>
+      <c r="AJ20" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="AK20" s="10" t="s">
         <v>12</v>
@@ -2767,20 +2670,11 @@
       <c r="AL20" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AM20" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AN20" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AO20" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AP20" s="10" t="s">
+      <c r="AM20" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="2:42" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:39" x14ac:dyDescent="0.4">
       <c r="C21" s="3">
         <v>5</v>
       </c>
@@ -2848,18 +2742,27 @@
       <c r="X21" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AE21" s="3">
+      <c r="AB21" s="3">
         <v>5</v>
       </c>
-      <c r="AF21" s="13">
+      <c r="AC21" s="13">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
+      <c r="AD21" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE21" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF21" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AG21" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AH21" s="10" t="s">
-        <v>12</v>
+      <c r="AH21" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="AI21" s="10" t="s">
         <v>12</v>
@@ -2867,8 +2770,8 @@
       <c r="AJ21" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AK21" s="9" t="s">
-        <v>11</v>
+      <c r="AK21" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AL21" s="10" t="s">
         <v>12</v>
@@ -2876,17 +2779,8 @@
       <c r="AM21" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AN21" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AO21" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AP21" s="10" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="22" spans="2:42" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:39" x14ac:dyDescent="0.4">
       <c r="C22" s="3">
         <v>6</v>
       </c>
@@ -2954,18 +2848,27 @@
       <c r="X22" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AE22" s="3">
+      <c r="AB22" s="3">
         <v>6</v>
       </c>
-      <c r="AF22" s="13">
+      <c r="AC22" s="13">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
+      <c r="AD22" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE22" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF22" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AG22" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AH22" s="10" t="s">
-        <v>12</v>
+      <c r="AH22" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="AI22" s="10" t="s">
         <v>12</v>
@@ -2973,8 +2876,8 @@
       <c r="AJ22" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AK22" s="9" t="s">
-        <v>11</v>
+      <c r="AK22" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AL22" s="10" t="s">
         <v>12</v>
@@ -2982,17 +2885,8 @@
       <c r="AM22" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AN22" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AO22" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AP22" s="10" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="23" spans="2:42" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:39" x14ac:dyDescent="0.4">
       <c r="C23" s="3">
         <v>7</v>
       </c>
@@ -3060,13 +2954,22 @@
       <c r="X23" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AE23" s="3">
+      <c r="AB23" s="3">
         <v>7</v>
       </c>
-      <c r="AF23" s="13">
+      <c r="AC23" s="13">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
+      <c r="AD23" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE23" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF23" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AG23" s="10" t="s">
         <v>12</v>
       </c>
@@ -3088,17 +2991,8 @@
       <c r="AM23" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AN23" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AO23" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AP23" s="10" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="24" spans="2:42" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:39" x14ac:dyDescent="0.4">
       <c r="C24" s="3">
         <v>8</v>
       </c>
@@ -3166,13 +3060,22 @@
       <c r="X24" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AE24" s="3">
+      <c r="AB24" s="3">
         <v>8</v>
       </c>
-      <c r="AF24" s="13">
+      <c r="AC24" s="13">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
+      <c r="AD24" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE24" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF24" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AG24" s="10" t="s">
         <v>12</v>
       </c>
@@ -3194,17 +3097,8 @@
       <c r="AM24" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AN24" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AO24" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AP24" s="10" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="25" spans="2:42" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:39" x14ac:dyDescent="0.4">
       <c r="C25" s="3">
         <v>9</v>
       </c>
@@ -3272,13 +3166,22 @@
       <c r="X25" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AE25" s="3">
+      <c r="AB25" s="3">
         <v>9</v>
       </c>
-      <c r="AF25" s="13">
+      <c r="AC25" s="13">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
+      <c r="AD25" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE25" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF25" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AG25" s="10" t="s">
         <v>12</v>
       </c>
@@ -3288,8 +3191,8 @@
       <c r="AI25" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AJ25" s="10" t="s">
-        <v>12</v>
+      <c r="AJ25" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="AK25" s="10" t="s">
         <v>12</v>
@@ -3297,20 +3200,11 @@
       <c r="AL25" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AM25" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AN25" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AO25" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AP25" s="10" t="s">
+      <c r="AM25" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="2:42" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:39" x14ac:dyDescent="0.4">
       <c r="C26" s="3">
         <v>10</v>
       </c>
@@ -3378,21 +3272,30 @@
       <c r="X26" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AE26" s="3">
+      <c r="AB26" s="3">
         <v>10</v>
       </c>
-      <c r="AF26" s="13">
+      <c r="AC26" s="13">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
+      <c r="AD26" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE26" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF26" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="AG26" s="10" t="s">
         <v>12</v>
       </c>
       <c r="AH26" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AI26" s="9" t="s">
-        <v>11</v>
+      <c r="AI26" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AJ26" s="10" t="s">
         <v>12</v>
@@ -3406,17 +3309,8 @@
       <c r="AM26" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AN26" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AO26" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AP26" s="10" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="27" spans="2:42" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:39" x14ac:dyDescent="0.4">
       <c r="C27" s="3">
         <v>11</v>
       </c>
@@ -3484,13 +3378,22 @@
       <c r="X27" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AE27" s="3">
-        <v>11</v>
-      </c>
-      <c r="AF27" s="13">
+      <c r="AB27" s="3">
+        <v>11</v>
+      </c>
+      <c r="AC27" s="13">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
+      <c r="AD27" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE27" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF27" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AG27" s="10" t="s">
         <v>12</v>
       </c>
@@ -3512,17 +3415,8 @@
       <c r="AM27" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AN27" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AO27" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AP27" s="10" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="28" spans="2:42" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:39" x14ac:dyDescent="0.4">
       <c r="C28" s="3">
         <v>12</v>
       </c>
@@ -3590,13 +3484,22 @@
       <c r="X28" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AE28" s="3">
-        <v>12</v>
-      </c>
-      <c r="AF28" s="13">
+      <c r="AB28" s="3">
+        <v>12</v>
+      </c>
+      <c r="AC28" s="13">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
+      <c r="AD28" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE28" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF28" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AG28" s="10" t="s">
         <v>12</v>
       </c>
@@ -3618,17 +3521,8 @@
       <c r="AM28" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AN28" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AO28" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AP28" s="10" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="29" spans="2:42" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:39" x14ac:dyDescent="0.4">
       <c r="C29" s="3">
         <v>13</v>
       </c>
@@ -3696,45 +3590,45 @@
       <c r="X29" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AE29" s="3">
+      <c r="AB29" s="3">
         <v>13</v>
       </c>
-      <c r="AF29" s="13">
+      <c r="AC29" s="13">
         <f t="shared" si="1"/>
         <v>0.7</v>
       </c>
+      <c r="AD29" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE29" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF29" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AG29" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AH29" s="10" t="s">
-        <v>12</v>
+      <c r="AH29" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="AI29" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AJ29" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AK29" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AL29" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AM29" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AN29" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AO29" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AP29" s="10" t="s">
+      <c r="AJ29" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AK29" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL29" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AM29" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="2:42" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:39" x14ac:dyDescent="0.4">
       <c r="C30" s="3">
         <v>14</v>
       </c>
@@ -3802,18 +3696,27 @@
       <c r="X30" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="AE30" s="3">
+      <c r="AB30" s="3">
         <v>14</v>
       </c>
-      <c r="AF30" s="13">
+      <c r="AC30" s="13">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
+      <c r="AD30" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE30" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF30" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AG30" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AH30" s="10" t="s">
-        <v>12</v>
+      <c r="AH30" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="AI30" s="10" t="s">
         <v>12</v>
@@ -3821,8 +3724,8 @@
       <c r="AJ30" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AK30" s="9" t="s">
-        <v>11</v>
+      <c r="AK30" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="AL30" s="10" t="s">
         <v>12</v>
@@ -3830,17 +3733,8 @@
       <c r="AM30" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AN30" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AO30" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AP30" s="10" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="31" spans="2:42" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:39" x14ac:dyDescent="0.4">
       <c r="D31" s="5"/>
       <c r="E31" s="16">
         <f>(COUNTIF(E17:E30,"○"))/14</f>
@@ -3922,16 +3816,25 @@
         <f t="shared" si="4"/>
         <v>7.1428571428571425E-2</v>
       </c>
-      <c r="AD31" s="3" t="s">
+      <c r="AA31" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="AE31" s="3">
+      <c r="AB31" s="3">
         <v>1</v>
       </c>
-      <c r="AF31" s="13">
+      <c r="AC31" s="13">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
+      <c r="AD31" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE31" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF31" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AG31" s="10" t="s">
         <v>12</v>
       </c>
@@ -3941,8 +3844,8 @@
       <c r="AI31" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AJ31" s="10" t="s">
-        <v>12</v>
+      <c r="AJ31" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="AK31" s="10" t="s">
         <v>12</v>
@@ -3950,32 +3853,32 @@
       <c r="AL31" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AM31" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AN31" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AO31" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AP31" s="10" t="s">
+      <c r="AM31" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="2:42" x14ac:dyDescent="0.4">
-      <c r="AE32" s="3">
+    <row r="32" spans="2:39" x14ac:dyDescent="0.4">
+      <c r="AB32" s="3">
         <v>2</v>
       </c>
-      <c r="AF32" s="13">
+      <c r="AC32" s="13">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
+      <c r="AD32" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE32" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF32" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AG32" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AH32" s="10" t="s">
-        <v>12</v>
+      <c r="AH32" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="AI32" s="10" t="s">
         <v>12</v>
@@ -3983,36 +3886,36 @@
       <c r="AJ32" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AK32" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AL32" s="10" t="s">
-        <v>12</v>
+      <c r="AK32" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AL32" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="AM32" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AN32" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AO32" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AP32" s="10" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="33" spans="30:42" x14ac:dyDescent="0.4">
-      <c r="AD33" s="3" t="s">
+    <row r="33" spans="27:39" x14ac:dyDescent="0.4">
+      <c r="AA33" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="AE33" s="3">
+      <c r="AB33" s="3">
         <v>1</v>
       </c>
-      <c r="AF33" s="13">
+      <c r="AC33" s="13">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
+      <c r="AD33" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE33" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF33" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AG33" s="10" t="s">
         <v>12</v>
       </c>
@@ -4034,24 +3937,24 @@
       <c r="AM33" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AN33" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AO33" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AP33" s="10" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="34" spans="30:42" x14ac:dyDescent="0.4">
-      <c r="AE34" s="3">
+    <row r="34" spans="27:39" x14ac:dyDescent="0.4">
+      <c r="AB34" s="3">
         <v>2</v>
       </c>
-      <c r="AF34" s="13">
+      <c r="AC34" s="13">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
+      <c r="AD34" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE34" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF34" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AG34" s="10" t="s">
         <v>12</v>
       </c>
@@ -4061,8 +3964,8 @@
       <c r="AI34" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AJ34" s="10" t="s">
-        <v>12</v>
+      <c r="AJ34" s="9" t="s">
+        <v>11</v>
       </c>
       <c r="AK34" s="10" t="s">
         <v>12</v>
@@ -4070,27 +3973,27 @@
       <c r="AL34" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AM34" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AN34" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AO34" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AP34" s="10" t="s">
+      <c r="AM34" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="30:42" x14ac:dyDescent="0.4">
-      <c r="AE35" s="3">
+    <row r="35" spans="27:39" x14ac:dyDescent="0.4">
+      <c r="AB35" s="3">
         <v>3</v>
       </c>
-      <c r="AF35" s="13">
+      <c r="AC35" s="13">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
+      <c r="AD35" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE35" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF35" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AG35" s="10" t="s">
         <v>12</v>
       </c>
@@ -4106,33 +4009,33 @@
       <c r="AK35" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AL35" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AM35" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AN35" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AO35" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="AP35" s="9" t="s">
+      <c r="AL35" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="AM35" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="36" spans="30:42" x14ac:dyDescent="0.4">
-      <c r="AD36" s="3" t="s">
+    <row r="36" spans="27:39" x14ac:dyDescent="0.4">
+      <c r="AA36" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="AE36" s="3">
+      <c r="AB36" s="3">
         <v>1</v>
       </c>
-      <c r="AF36" s="13">
+      <c r="AC36" s="13">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
+      <c r="AD36" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE36" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF36" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="AG36" s="10" t="s">
         <v>12</v>
       </c>
@@ -4154,54 +4057,45 @@
       <c r="AM36" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AN36" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AO36" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AP36" s="10" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="37" spans="30:42" x14ac:dyDescent="0.4">
+    <row r="37" spans="27:39" x14ac:dyDescent="0.4">
+      <c r="AD37" s="16">
+        <f>(COUNTIF(AD3:AD36,"○")/32)</f>
+        <v>1</v>
+      </c>
+      <c r="AE37" s="16">
+        <f t="shared" ref="AE37:AM37" si="5">(COUNTIF(AE3:AE36,"○")/32)</f>
+        <v>0.9375</v>
+      </c>
+      <c r="AF37" s="16">
+        <f t="shared" si="5"/>
+        <v>0.9375</v>
+      </c>
       <c r="AG37" s="16">
-        <f>(COUNTIF(AG3:AG36,"○")/32)</f>
-        <v>1</v>
+        <f t="shared" si="5"/>
+        <v>0.96875</v>
       </c>
       <c r="AH37" s="16">
-        <f t="shared" ref="AH37:AP37" si="5">(COUNTIF(AH3:AH36,"○")/32)</f>
-        <v>0.9375</v>
+        <f t="shared" si="5"/>
+        <v>0.59375</v>
       </c>
       <c r="AI37" s="16">
         <f t="shared" si="5"/>
-        <v>0.9375</v>
+        <v>0.875</v>
       </c>
       <c r="AJ37" s="16">
         <f t="shared" si="5"/>
-        <v>0.96875</v>
+        <v>0.5625</v>
       </c>
       <c r="AK37" s="16">
         <f t="shared" si="5"/>
-        <v>0.59375</v>
+        <v>1</v>
       </c>
       <c r="AL37" s="16">
         <f t="shared" si="5"/>
         <v>0.875</v>
       </c>
       <c r="AM37" s="16">
-        <f t="shared" si="5"/>
-        <v>0.5625</v>
-      </c>
-      <c r="AN37" s="16">
-        <f t="shared" si="5"/>
-        <v>1</v>
-      </c>
-      <c r="AO37" s="16">
-        <f t="shared" si="5"/>
-        <v>0.875</v>
-      </c>
-      <c r="AP37" s="16">
         <f t="shared" si="5"/>
         <v>0.9375</v>
       </c>
@@ -4209,7 +4103,7 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="E1:X1"/>
-    <mergeCell ref="AG1:AP1"/>
+    <mergeCell ref="AD1:AM1"/>
   </mergeCells>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>